<commit_message>
Updating and correcting data
Added commercial harvest for 2018-2020. Added FSC harvest 2018-2020. Corrected Commercial harvest for 2017 caught/releases.
</commit_message>
<xml_diff>
--- a/data/harvest/misc/Area 8 potential sx interception.xlsx
+++ b/data/harvest/misc/Area 8 potential sx interception.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CONNORSB\Documents\Github\Atnarko-sockeye\data\harvest\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_GitHub\Atnarko-sockeye\data\harvest\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5E61299-D1F4-4904-A95A-63C53044E3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3213EDB-3D20-4D4D-8608-832356F3662D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28755" yWindow="-2520" windowWidth="14145" windowHeight="14775" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Commercial!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="203">
   <si>
     <t>TARGET SPECIES</t>
   </si>
@@ -616,12 +616,117 @@
   </si>
   <si>
     <t>*PSR documents are typically preliminary, RMS documents are more final</t>
+  </si>
+  <si>
+    <t>2018 PSR</t>
+  </si>
+  <si>
+    <t>8-3, 8-4, 8-5</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Sx caught b/w July 8 and July 28</t>
+  </si>
+  <si>
+    <t>37 sx rel</t>
+  </si>
+  <si>
+    <t>DFO 2018 Post Season Review</t>
+  </si>
+  <si>
+    <t>205 sx rel</t>
+  </si>
+  <si>
+    <t>4296 sx rel</t>
+  </si>
+  <si>
+    <t>DFO 2019 Post Season Review</t>
+  </si>
+  <si>
+    <t>0 sx rel</t>
+  </si>
+  <si>
+    <t>26 sx rel</t>
+  </si>
+  <si>
+    <t>459 sx rel</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>2019 PSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> June</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>update gear?</t>
+  </si>
+  <si>
+    <t>sx caught b/w June 16 - July 27</t>
+  </si>
+  <si>
+    <t>8-3, 8-4, 8-5, PSR states incomplete (try to track down</t>
+  </si>
+  <si>
+    <t>follow-up</t>
+  </si>
+  <si>
+    <t>DFO 2020 Post Season Review</t>
+  </si>
+  <si>
+    <t>4 sx rel, COVID-19 limited openings</t>
+  </si>
+  <si>
+    <t>0 sx rel, COVID-19 limited openings</t>
+  </si>
+  <si>
+    <t>23 sx rel, COVID-19 limited openings</t>
+  </si>
+  <si>
+    <t>72 sx rel, COVID019 limited openings</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>8-3, 8-4, 8-5 (COVID-19)</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>sx caught b/w June 16 - Aug 3,Does not separate DN upper and lower Bella Coola</t>
+  </si>
+  <si>
+    <t>Sx caught b/w June 17 - Aug 4, Does not separate DN upper and lower Bella Coola</t>
+  </si>
+  <si>
+    <t>Sx caught b/w June 14 and Aug 8, Does not separate DN upper and lower Bella Coola, COVID-19</t>
+  </si>
+  <si>
+    <t>2020 PSR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -682,12 +787,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -957,7 +1068,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1126,23 +1237,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1155,6 +1254,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="227">
@@ -1721,10 +1853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:H69"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1792,10 +1925,10 @@
       <c r="C5" s="51">
         <v>43339</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="69">
         <v>27</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="69" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="23" t="s">
@@ -1822,8 +1955,8 @@
       <c r="C6" s="22">
         <v>43326</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
       <c r="F6" s="23" t="s">
         <v>49</v>
       </c>
@@ -1845,7 +1978,7 @@
         <v>43339</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="E7" s="71"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="23" t="s">
         <v>13</v>
       </c>
@@ -1894,10 +2027,10 @@
       <c r="C9" s="33">
         <v>43345</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="72">
         <v>29</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="72" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="34" t="s">
@@ -1924,8 +2057,8 @@
       <c r="C10" s="37">
         <v>43345</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="38" t="s">
         <v>24</v>
       </c>
@@ -1946,8 +2079,8 @@
       <c r="C11" s="37">
         <v>43334</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="38" t="s">
         <v>12</v>
       </c>
@@ -1996,10 +2129,10 @@
       <c r="C13" s="33">
         <v>43344</v>
       </c>
-      <c r="D13" s="76">
+      <c r="D13" s="72">
         <v>28</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="72" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="34" t="s">
@@ -2026,8 +2159,8 @@
       <c r="C14" s="37">
         <v>43344</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="38" t="s">
         <v>24</v>
       </c>
@@ -2048,8 +2181,8 @@
       <c r="C15" s="37">
         <v>43338</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="38" t="s">
         <v>12</v>
       </c>
@@ -2098,10 +2231,10 @@
       <c r="C17" s="17">
         <v>43343</v>
       </c>
-      <c r="D17" s="70">
+      <c r="D17" s="68">
         <v>28</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="34" t="s">
@@ -2128,8 +2261,8 @@
       <c r="C18" s="51">
         <v>43343</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="38" t="s">
         <v>24</v>
       </c>
@@ -2150,8 +2283,8 @@
       <c r="C19" s="4">
         <v>43343</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="38" t="s">
         <v>12</v>
       </c>
@@ -2199,10 +2332,10 @@
       <c r="C21" s="18">
         <v>43334</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="68">
         <v>21</v>
       </c>
-      <c r="E21" s="70" t="s">
+      <c r="E21" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="34" t="s">
@@ -2229,8 +2362,8 @@
       <c r="C22" s="51">
         <v>43334</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="38" t="s">
         <v>24</v>
       </c>
@@ -2251,8 +2384,8 @@
       <c r="C23" s="51">
         <v>43334</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="38" t="s">
         <v>12</v>
       </c>
@@ -2300,10 +2433,10 @@
       <c r="C25" s="18">
         <v>43340</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="68">
         <v>24</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F25" s="34" t="s">
@@ -2315,7 +2448,7 @@
       <c r="H25" s="50">
         <v>45</v>
       </c>
-      <c r="I25" s="74" t="s">
+      <c r="I25" s="70" t="s">
         <v>21</v>
       </c>
       <c r="J25" s="50" t="s">
@@ -2330,8 +2463,8 @@
       <c r="C26" s="51">
         <v>43340</v>
       </c>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="38" t="s">
         <v>24</v>
       </c>
@@ -2341,7 +2474,7 @@
       <c r="H26" s="39">
         <v>2</v>
       </c>
-      <c r="I26" s="75"/>
+      <c r="I26" s="71"/>
       <c r="J26" s="24"/>
     </row>
     <row r="27" spans="1:10">
@@ -2352,7 +2485,7 @@
       <c r="C27" s="51">
         <v>43340</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="69"/>
       <c r="E27" s="26"/>
       <c r="F27" s="38" t="s">
         <v>12</v>
@@ -2401,10 +2534,10 @@
       <c r="C29" s="18">
         <v>43325</v>
       </c>
-      <c r="D29" s="70">
+      <c r="D29" s="68">
         <v>18</v>
       </c>
-      <c r="E29" s="70" t="s">
+      <c r="E29" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="34" t="s">
@@ -2431,8 +2564,8 @@
       <c r="C30" s="51">
         <v>43325</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
       <c r="F30" s="38" t="s">
         <v>24</v>
       </c>
@@ -2453,8 +2586,8 @@
       <c r="C31" s="51">
         <v>43325</v>
       </c>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="38" t="s">
         <v>12</v>
       </c>
@@ -2502,10 +2635,10 @@
       <c r="C33" s="18">
         <v>43302</v>
       </c>
-      <c r="D33" s="70">
+      <c r="D33" s="68">
         <v>6</v>
       </c>
-      <c r="E33" s="70" t="s">
+      <c r="E33" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F33" s="34" t="s">
@@ -2517,7 +2650,7 @@
       <c r="H33" s="50">
         <v>13</v>
       </c>
-      <c r="I33" s="68" t="s">
+      <c r="I33" s="74" t="s">
         <v>114</v>
       </c>
       <c r="J33" s="20" t="s">
@@ -2532,8 +2665,8 @@
       <c r="C34" s="51">
         <v>43302</v>
       </c>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="38" t="s">
         <v>12</v>
       </c>
@@ -2543,7 +2676,7 @@
       <c r="H34" s="39">
         <v>184</v>
       </c>
-      <c r="I34" s="69"/>
+      <c r="I34" s="75"/>
       <c r="J34" s="25"/>
     </row>
     <row r="35" spans="1:10">
@@ -2569,7 +2702,7 @@
       <c r="H35" s="39">
         <v>197</v>
       </c>
-      <c r="I35" s="69"/>
+      <c r="I35" s="75"/>
       <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10">
@@ -2582,10 +2715,10 @@
       <c r="C36" s="18">
         <v>43316</v>
       </c>
-      <c r="D36" s="70">
+      <c r="D36" s="68">
         <v>12</v>
       </c>
-      <c r="E36" s="70" t="s">
+      <c r="E36" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="34" t="s">
@@ -2610,8 +2743,8 @@
       <c r="C37" s="51">
         <v>43320</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
       <c r="F37" s="38" t="s">
         <v>24</v>
       </c>
@@ -2632,8 +2765,8 @@
       <c r="C38" s="51">
         <v>43316</v>
       </c>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="38" t="s">
         <v>12</v>
       </c>
@@ -2681,10 +2814,10 @@
       <c r="C40" s="18">
         <v>43307</v>
       </c>
-      <c r="D40" s="70">
+      <c r="D40" s="68">
         <v>6</v>
       </c>
-      <c r="E40" s="70" t="s">
+      <c r="E40" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="34" t="s">
@@ -2696,7 +2829,7 @@
       <c r="H40" s="50">
         <v>32</v>
       </c>
-      <c r="I40" s="72" t="s">
+      <c r="I40" s="76" t="s">
         <v>26</v>
       </c>
       <c r="J40" s="58" t="s">
@@ -2711,8 +2844,8 @@
       <c r="C41" s="51">
         <v>43307</v>
       </c>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="38" t="s">
         <v>12</v>
       </c>
@@ -2722,7 +2855,7 @@
       <c r="H41" s="39">
         <v>268</v>
       </c>
-      <c r="I41" s="73"/>
+      <c r="I41" s="77"/>
       <c r="J41" s="59"/>
     </row>
     <row r="42" spans="1:10">
@@ -2746,7 +2879,7 @@
         <v>16</v>
       </c>
       <c r="H42" s="24"/>
-      <c r="I42" s="73"/>
+      <c r="I42" s="77"/>
       <c r="J42" s="59"/>
     </row>
     <row r="43" spans="1:10" ht="31.5">
@@ -2759,10 +2892,10 @@
       <c r="C43" s="18">
         <v>43344</v>
       </c>
-      <c r="D43" s="70">
+      <c r="D43" s="68">
         <v>14</v>
       </c>
-      <c r="E43" s="70" t="s">
+      <c r="E43" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F43" s="34" t="s">
@@ -2789,8 +2922,8 @@
       <c r="C44" s="51">
         <v>43335</v>
       </c>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="38" t="s">
         <v>24</v>
       </c>
@@ -2811,8 +2944,8 @@
       <c r="C45" s="51">
         <v>43344</v>
       </c>
-      <c r="D45" s="71"/>
-      <c r="E45" s="71"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
       <c r="F45" s="38" t="s">
         <v>12</v>
       </c>
@@ -2863,10 +2996,10 @@
       <c r="C47" s="18">
         <v>43325</v>
       </c>
-      <c r="D47" s="70">
+      <c r="D47" s="68">
         <v>16</v>
       </c>
-      <c r="E47" s="70" t="s">
+      <c r="E47" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F47" s="34" t="s">
@@ -2893,8 +3026,8 @@
       <c r="C48" s="51">
         <v>43325</v>
       </c>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="38" t="s">
         <v>24</v>
       </c>
@@ -2915,8 +3048,8 @@
       <c r="C49" s="51">
         <v>43325</v>
       </c>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
       <c r="F49" s="38" t="s">
         <v>12</v>
       </c>
@@ -2967,10 +3100,10 @@
       <c r="C51" s="18">
         <v>43338</v>
       </c>
-      <c r="D51" s="70">
+      <c r="D51" s="68">
         <v>17</v>
       </c>
-      <c r="E51" s="70" t="s">
+      <c r="E51" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F51" s="34" t="s">
@@ -2997,8 +3130,8 @@
       <c r="C52" s="51">
         <v>43331</v>
       </c>
-      <c r="D52" s="71"/>
-      <c r="E52" s="71"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
       <c r="F52" s="38" t="s">
         <v>24</v>
       </c>
@@ -3021,8 +3154,8 @@
       <c r="C53" s="51">
         <v>43338</v>
       </c>
-      <c r="D53" s="71"/>
-      <c r="E53" s="71"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
       <c r="F53" s="38" t="s">
         <v>12</v>
       </c>
@@ -3074,10 +3207,10 @@
       <c r="C55" s="18">
         <v>43316</v>
       </c>
-      <c r="D55" s="70">
+      <c r="D55" s="68">
         <v>11</v>
       </c>
-      <c r="E55" s="70" t="s">
+      <c r="E55" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F55" s="34" t="s">
@@ -3104,8 +3237,8 @@
       <c r="C56" s="51">
         <v>43316</v>
       </c>
-      <c r="D56" s="71"/>
-      <c r="E56" s="71"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
       <c r="F56" s="38" t="s">
         <v>12</v>
       </c>
@@ -3158,10 +3291,10 @@
       <c r="C58" s="18">
         <v>43330</v>
       </c>
-      <c r="D58" s="70">
+      <c r="D58" s="68">
         <v>19</v>
       </c>
-      <c r="E58" s="70" t="s">
+      <c r="E58" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F58" s="34" t="s">
@@ -3188,8 +3321,8 @@
       <c r="C59" s="51">
         <v>43322</v>
       </c>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="69"/>
       <c r="F59" s="38" t="s">
         <v>24</v>
       </c>
@@ -3212,8 +3345,8 @@
       <c r="C60" s="51">
         <v>43330</v>
       </c>
-      <c r="D60" s="71"/>
-      <c r="E60" s="71"/>
+      <c r="D60" s="69"/>
+      <c r="E60" s="69"/>
       <c r="F60" s="38" t="s">
         <v>12</v>
       </c>
@@ -3266,10 +3399,10 @@
       <c r="C62" s="18">
         <v>43334</v>
       </c>
-      <c r="D62" s="70">
+      <c r="D62" s="68">
         <v>16</v>
       </c>
-      <c r="E62" s="70" t="s">
+      <c r="E62" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F62" s="34" t="s">
@@ -3296,8 +3429,8 @@
       <c r="C63" s="51">
         <v>43320</v>
       </c>
-      <c r="D63" s="71"/>
-      <c r="E63" s="71"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="69"/>
       <c r="F63" s="38" t="s">
         <v>24</v>
       </c>
@@ -3320,8 +3453,8 @@
       <c r="C64" s="51">
         <v>43320</v>
       </c>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
+      <c r="D64" s="69"/>
+      <c r="E64" s="69"/>
       <c r="F64" s="38" t="s">
         <v>12</v>
       </c>
@@ -3374,10 +3507,10 @@
       <c r="C66" s="18">
         <v>43327</v>
       </c>
-      <c r="D66" s="70">
+      <c r="D66" s="68">
         <v>16</v>
       </c>
-      <c r="E66" s="70" t="s">
+      <c r="E66" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F66" s="34" t="s">
@@ -3404,8 +3537,8 @@
       <c r="C67" s="51">
         <v>43319</v>
       </c>
-      <c r="D67" s="71"/>
-      <c r="E67" s="71"/>
+      <c r="D67" s="69"/>
+      <c r="E67" s="69"/>
       <c r="F67" s="38" t="s">
         <v>24</v>
       </c>
@@ -3428,8 +3561,8 @@
       <c r="C68" s="51">
         <v>43327</v>
       </c>
-      <c r="D68" s="71"/>
-      <c r="E68" s="71"/>
+      <c r="D68" s="69"/>
+      <c r="E68" s="69"/>
       <c r="F68" s="23" t="s">
         <v>12</v>
       </c>
@@ -3473,45 +3606,386 @@
       <c r="J69" s="67"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="E70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="I70" s="9"/>
+      <c r="A70">
+        <v>2018</v>
+      </c>
+      <c r="B70" s="79">
+        <v>43255</v>
+      </c>
+      <c r="C70" s="79">
+        <v>43326</v>
+      </c>
+      <c r="D70" s="39">
+        <v>14</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70">
+        <f>547+37</f>
+        <v>584</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J70" s="38" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="E71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="I71" s="9"/>
+      <c r="B71" s="79">
+        <v>43297</v>
+      </c>
+      <c r="C71" s="80">
+        <v>43326</v>
+      </c>
+      <c r="D71" s="39">
+        <v>7</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71">
+        <f>69+1</f>
+        <v>70</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="G72" s="1"/>
-      <c r="I72" s="9"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="81">
+        <v>43283</v>
+      </c>
+      <c r="C72" s="81">
+        <v>43326</v>
+      </c>
+      <c r="D72" s="39">
+        <v>10</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="24">
+        <f>2947+205</f>
+        <v>3152</v>
+      </c>
+      <c r="I72" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J72" s="24"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="G73" s="1"/>
-      <c r="I73" s="9"/>
+      <c r="A73" s="29"/>
+      <c r="B73" s="82">
+        <v>43297</v>
+      </c>
+      <c r="C73" s="83">
+        <v>43326</v>
+      </c>
+      <c r="D73" s="42">
+        <v>7</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73" s="29">
+        <f>0+4296</f>
+        <v>4296</v>
+      </c>
+      <c r="I73" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="J73" s="29"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="G74" s="1"/>
-      <c r="I74" s="9"/>
+      <c r="A74" s="50">
+        <v>2019</v>
+      </c>
+      <c r="B74" s="84">
+        <v>43619</v>
+      </c>
+      <c r="C74" s="84">
+        <v>43680</v>
+      </c>
+      <c r="D74" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="50">
+        <f>29+5</f>
+        <v>34</v>
+      </c>
+      <c r="I74" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="19" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="75" spans="1:10">
-      <c r="G75" s="1"/>
-      <c r="I75" s="9"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="81">
+        <v>43660</v>
+      </c>
+      <c r="C75" s="80">
+        <v>43680</v>
+      </c>
+      <c r="D75" s="86" t="s">
+        <v>181</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F75" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="24">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="I75" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="J75" s="24"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="G76" s="1"/>
-      <c r="I76" s="9"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="80">
+        <v>43647</v>
+      </c>
+      <c r="C76" s="81">
+        <v>43680</v>
+      </c>
+      <c r="D76" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="24">
+        <f>247+26</f>
+        <v>273</v>
+      </c>
+      <c r="I76" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J76" s="24"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="G77" s="1"/>
-      <c r="I77" s="9"/>
+      <c r="A77" s="29"/>
+      <c r="B77" s="82">
+        <v>43661</v>
+      </c>
+      <c r="C77" s="83">
+        <v>43680</v>
+      </c>
+      <c r="D77" s="29">
+        <v>2</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" s="29">
+        <v>459</v>
+      </c>
+      <c r="I77" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="J77" s="29"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="G78" s="1"/>
-      <c r="I78" s="9"/>
+      <c r="A78">
+        <v>2020</v>
+      </c>
+      <c r="B78" s="79">
+        <v>43997</v>
+      </c>
+      <c r="C78" s="79">
+        <v>44032</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78">
+        <f>11 + 4</f>
+        <v>15</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="J78" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="B79" s="79">
+        <v>44032</v>
+      </c>
+      <c r="C79" s="79">
+        <v>44032</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="24"/>
+      <c r="B80" s="81">
+        <v>44015</v>
+      </c>
+      <c r="C80" s="81">
+        <v>44032</v>
+      </c>
+      <c r="D80" s="24">
+        <v>3</v>
+      </c>
+      <c r="E80" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F80" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="24">
+        <f>199+23</f>
+        <v>222</v>
+      </c>
+      <c r="I80" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="J80" s="24"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="29"/>
+      <c r="B81" s="82">
+        <v>44032</v>
+      </c>
+      <c r="C81" s="82">
+        <v>44032</v>
+      </c>
+      <c r="D81" s="29">
+        <v>1</v>
+      </c>
+      <c r="E81" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="29">
+        <v>72</v>
+      </c>
+      <c r="I81" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="J81" s="29"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="E82" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="E66:E68"/>
     <mergeCell ref="D66:D68"/>
     <mergeCell ref="D25:D27"/>
@@ -3526,29 +4000,6 @@
     <mergeCell ref="E58:E60"/>
     <mergeCell ref="E62:E64"/>
     <mergeCell ref="D62:D64"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3564,10 +4015,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <pane ySplit="4" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3580,7 +4032,7 @@
     <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -3588,7 +4040,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="48" thickBot="1">
+    <row r="4" spans="1:11" ht="48" thickBot="1">
       <c r="A4" s="56" t="s">
         <v>1</v>
       </c>
@@ -3619,8 +4071,11 @@
       <c r="J4" s="57" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="6" customFormat="1">
+      <c r="K4" s="88" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1">
       <c r="A5" s="15">
         <v>2001</v>
       </c>
@@ -3652,7 +4107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="B6" s="4">
         <v>43208</v>
@@ -3682,7 +4137,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="4">
         <v>43258</v>
@@ -3712,7 +4167,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="B8" s="4">
         <v>43258</v>
@@ -3742,7 +4197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="16">
         <v>2002</v>
       </c>
@@ -3774,7 +4229,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="2"/>
       <c r="B10" s="4">
         <v>43210</v>
@@ -3804,7 +4259,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="2"/>
       <c r="B11" s="4">
         <v>43259</v>
@@ -3834,7 +4289,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="B12" s="4">
         <v>43259</v>
@@ -3864,7 +4319,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="16">
         <v>2003</v>
       </c>
@@ -3896,7 +4351,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="2"/>
       <c r="B14" s="4">
         <v>43209</v>
@@ -3926,7 +4381,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="2"/>
       <c r="B15" s="4">
         <v>43258</v>
@@ -3956,7 +4411,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="B16" s="4">
         <v>43259</v>
@@ -4457,7 +4912,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:11">
       <c r="A33" s="2"/>
       <c r="B33" s="4">
         <v>43211</v>
@@ -4486,8 +4941,11 @@
       <c r="J33" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="2"/>
       <c r="B34" s="4">
         <v>43211</v>
@@ -4517,7 +4975,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:11">
       <c r="A35" s="2"/>
       <c r="B35" s="4">
         <v>43253</v>
@@ -4547,7 +5005,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:11">
       <c r="A36" s="2"/>
       <c r="B36" s="4">
         <v>43253</v>
@@ -4577,7 +5035,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" s="16">
         <v>2008</v>
       </c>
@@ -4609,7 +5067,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="31.5">
+    <row r="38" spans="1:11" ht="31.5">
       <c r="A38" s="2"/>
       <c r="B38" s="4">
         <v>43209</v>
@@ -4639,7 +5097,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="A39" s="2"/>
       <c r="B39" s="4">
         <v>43209</v>
@@ -4669,7 +5127,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:11">
       <c r="A40" s="2"/>
       <c r="B40" s="4">
         <v>43286</v>
@@ -4699,7 +5157,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41" s="2"/>
       <c r="B41" s="4">
         <v>43272</v>
@@ -4729,7 +5187,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42" s="16">
         <v>2009</v>
       </c>
@@ -4761,7 +5219,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:11">
       <c r="A43" s="2"/>
       <c r="B43" s="4">
         <v>43208</v>
@@ -4791,7 +5249,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44" s="2"/>
       <c r="B44" s="4">
         <v>43208</v>
@@ -4821,7 +5279,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45" s="2"/>
       <c r="B45" s="4">
         <v>43278</v>
@@ -4851,7 +5309,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:11">
       <c r="A46" s="2"/>
       <c r="B46" s="4">
         <v>43278</v>
@@ -4881,7 +5339,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="31.5">
+    <row r="47" spans="1:11" ht="31.5">
       <c r="A47" s="16">
         <v>2010</v>
       </c>
@@ -4913,7 +5371,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48" s="2"/>
       <c r="B48" s="4">
         <v>43267</v>
@@ -5400,7 +5858,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:11">
       <c r="A65" s="2"/>
       <c r="B65" s="4">
         <v>43208</v>
@@ -5430,7 +5888,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:11">
       <c r="A66" s="50">
         <v>2016</v>
       </c>
@@ -5462,7 +5920,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:11">
       <c r="A67" s="2"/>
       <c r="B67" s="4">
         <v>43234</v>
@@ -5492,7 +5950,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:11">
       <c r="A68" s="2"/>
       <c r="B68" s="4">
         <v>43206</v>
@@ -5512,7 +5970,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:11">
       <c r="A69" s="50">
         <v>2017</v>
       </c>
@@ -5544,7 +6002,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:11">
       <c r="B70" s="4">
         <v>43247</v>
       </c>
@@ -5573,20 +6031,21 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
-      <c r="B71" s="4">
+    <row r="71" spans="1:11">
+      <c r="A71" s="24"/>
+      <c r="B71" s="51">
         <v>43261</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="51">
         <v>43345</v>
       </c>
       <c r="D71" s="39">
         <v>7</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="23" t="s">
         <v>145</v>
       </c>
       <c r="G71" s="39">
@@ -5598,68 +6057,349 @@
       <c r="I71" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="J71" s="21" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="50"/>
-      <c r="B72" s="18">
+    <row r="72" spans="1:11">
+      <c r="A72" s="29"/>
+      <c r="B72" s="66">
         <v>43212</v>
       </c>
-      <c r="C72" s="18">
+      <c r="C72" s="66">
         <v>43359</v>
       </c>
-      <c r="D72" s="35">
+      <c r="D72" s="42">
         <v>3</v>
       </c>
-      <c r="E72" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F72" s="19" t="s">
+      <c r="E72" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="G72" s="35">
+      <c r="G72" s="42">
         <v>320</v>
       </c>
-      <c r="H72" s="32" t="s">
+      <c r="H72" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I72" s="58"/>
-      <c r="J72" s="16" t="s">
+      <c r="I72" s="67"/>
+      <c r="J72" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>2018</v>
+      </c>
+      <c r="B73" s="79">
+        <v>43288</v>
+      </c>
+      <c r="C73" s="79">
+        <v>43330</v>
+      </c>
+      <c r="D73" s="39">
+        <v>7</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" s="39">
+        <v>0</v>
+      </c>
+      <c r="H73" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I73" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="J73" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="B74" s="79">
+        <v>43282</v>
+      </c>
+      <c r="C74" s="79">
+        <v>43386</v>
+      </c>
+      <c r="D74" s="39">
+        <v>7</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G74" s="39">
+        <v>1521</v>
+      </c>
+      <c r="H74" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I74" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="J74" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="B75" s="79">
+        <v>43240</v>
+      </c>
+      <c r="C75" s="79">
+        <v>43379</v>
+      </c>
+      <c r="D75" s="39">
+        <v>20</v>
+      </c>
+      <c r="E75" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F75" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G75" s="39">
+        <v>111</v>
+      </c>
+      <c r="H75" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I75" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="J75" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="29"/>
+      <c r="B76" s="82">
+        <v>43261</v>
+      </c>
+      <c r="C76" s="82">
+        <v>43316</v>
+      </c>
+      <c r="D76" s="42">
+        <v>5</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F76" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G76" s="42">
+        <v>8</v>
+      </c>
+      <c r="H76" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I76" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="J76" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>2019</v>
+      </c>
+      <c r="B77" s="79">
+        <v>43641</v>
+      </c>
+      <c r="C77" s="79">
+        <v>43678</v>
+      </c>
+      <c r="D77" s="39">
+        <v>3</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" s="39">
+        <v>0</v>
+      </c>
+      <c r="H77" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I77" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="J77" s="36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="B78" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="C78" s="79" t="s">
+        <v>184</v>
+      </c>
+      <c r="D78" t="s">
+        <v>181</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G78" s="39">
+        <v>71</v>
+      </c>
+      <c r="H78" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I78" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="J78" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="K78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="B79" s="80">
+        <v>43603</v>
+      </c>
+      <c r="C79" s="79">
+        <v>43680</v>
+      </c>
+      <c r="D79">
+        <v>10</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G79" s="39">
+        <v>57</v>
+      </c>
+      <c r="H79" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I79" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="J79" s="36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="29"/>
+      <c r="B80" s="82">
+        <v>43625</v>
+      </c>
+      <c r="C80" s="82">
+        <v>43673</v>
+      </c>
+      <c r="D80" s="29">
+        <v>6</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F80" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G80" s="42">
+        <v>34</v>
+      </c>
+      <c r="H80" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I80" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="J80" s="40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81">
+        <v>2020</v>
+      </c>
+      <c r="B81" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" t="s">
+        <v>181</v>
+      </c>
+      <c r="E81" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F81" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G81" s="39">
+        <v>571</v>
+      </c>
+      <c r="H81" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I81" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="J81" s="36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="29"/>
+      <c r="B82" s="82">
+        <v>44005</v>
+      </c>
+      <c r="C82" s="82">
+        <v>44058</v>
+      </c>
+      <c r="D82" s="29">
+        <v>12</v>
+      </c>
+      <c r="E82" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="F82" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="G82" s="42">
+        <v>37</v>
+      </c>
+      <c r="H82" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I82" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="J82" s="40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" t="s">
         <v>168</v>
       </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
KM updates from 4 months ago (#2)
* started ages

* Ages completed

finished manual extraction for BCR FSC data, marine harvest, and real (total age) structure data from excel file.

updated readme.

* Started genetics section

Unclear how to move forward with GSI data here.

* Rename age_subfolder_README.md to README.md

* Updating and correcting data

Added commercial harvest for 2018-2020. Added FSC harvest 2018-2020. Corrected Commercial harvest for 2017 caught/releases.

* added total spawners to date

data are highly uncertain. Many years do not include surveys of Atnarko River mainstem. Total estimates are derived from Above Stillwater lake (the first lake) any beyond.

* Adding 2024 total escapement

---------

Co-authored-by: kateaurora <katmcignvey@gmail.com>
</commit_message>
<xml_diff>
--- a/data/harvest/misc/Area 8 potential sx interception.xlsx
+++ b/data/harvest/misc/Area 8 potential sx interception.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CONNORSB\Documents\Github\Atnarko-sockeye\data\harvest\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_GitHub\Atnarko-sockeye\data\harvest\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5E61299-D1F4-4904-A95A-63C53044E3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3213EDB-3D20-4D4D-8608-832356F3662D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28755" yWindow="-2520" windowWidth="14145" windowHeight="14775" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commercial" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Commercial!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="203">
   <si>
     <t>TARGET SPECIES</t>
   </si>
@@ -616,12 +616,117 @@
   </si>
   <si>
     <t>*PSR documents are typically preliminary, RMS documents are more final</t>
+  </si>
+  <si>
+    <t>2018 PSR</t>
+  </si>
+  <si>
+    <t>8-3, 8-4, 8-5</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Sx caught b/w July 8 and July 28</t>
+  </si>
+  <si>
+    <t>37 sx rel</t>
+  </si>
+  <si>
+    <t>DFO 2018 Post Season Review</t>
+  </si>
+  <si>
+    <t>205 sx rel</t>
+  </si>
+  <si>
+    <t>4296 sx rel</t>
+  </si>
+  <si>
+    <t>DFO 2019 Post Season Review</t>
+  </si>
+  <si>
+    <t>0 sx rel</t>
+  </si>
+  <si>
+    <t>26 sx rel</t>
+  </si>
+  <si>
+    <t>459 sx rel</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>2019 PSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> June</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>update gear?</t>
+  </si>
+  <si>
+    <t>sx caught b/w June 16 - July 27</t>
+  </si>
+  <si>
+    <t>8-3, 8-4, 8-5, PSR states incomplete (try to track down</t>
+  </si>
+  <si>
+    <t>follow-up</t>
+  </si>
+  <si>
+    <t>DFO 2020 Post Season Review</t>
+  </si>
+  <si>
+    <t>4 sx rel, COVID-19 limited openings</t>
+  </si>
+  <si>
+    <t>0 sx rel, COVID-19 limited openings</t>
+  </si>
+  <si>
+    <t>23 sx rel, COVID-19 limited openings</t>
+  </si>
+  <si>
+    <t>72 sx rel, COVID019 limited openings</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>8-3, 8-4, 8-5 (COVID-19)</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>sx caught b/w June 16 - Aug 3,Does not separate DN upper and lower Bella Coola</t>
+  </si>
+  <si>
+    <t>Sx caught b/w June 17 - Aug 4, Does not separate DN upper and lower Bella Coola</t>
+  </si>
+  <si>
+    <t>Sx caught b/w June 14 and Aug 8, Does not separate DN upper and lower Bella Coola, COVID-19</t>
+  </si>
+  <si>
+    <t>2020 PSR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -682,12 +787,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -957,7 +1068,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1126,23 +1237,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1155,6 +1254,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="227">
@@ -1721,10 +1853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25:H69"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1792,10 +1925,10 @@
       <c r="C5" s="51">
         <v>43339</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="69">
         <v>27</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="69" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="23" t="s">
@@ -1822,8 +1955,8 @@
       <c r="C6" s="22">
         <v>43326</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
       <c r="F6" s="23" t="s">
         <v>49</v>
       </c>
@@ -1845,7 +1978,7 @@
         <v>43339</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="E7" s="71"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="23" t="s">
         <v>13</v>
       </c>
@@ -1894,10 +2027,10 @@
       <c r="C9" s="33">
         <v>43345</v>
       </c>
-      <c r="D9" s="76">
+      <c r="D9" s="72">
         <v>29</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="72" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="34" t="s">
@@ -1924,8 +2057,8 @@
       <c r="C10" s="37">
         <v>43345</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="38" t="s">
         <v>24</v>
       </c>
@@ -1946,8 +2079,8 @@
       <c r="C11" s="37">
         <v>43334</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
       <c r="F11" s="38" t="s">
         <v>12</v>
       </c>
@@ -1996,10 +2129,10 @@
       <c r="C13" s="33">
         <v>43344</v>
       </c>
-      <c r="D13" s="76">
+      <c r="D13" s="72">
         <v>28</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="72" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="34" t="s">
@@ -2026,8 +2159,8 @@
       <c r="C14" s="37">
         <v>43344</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="38" t="s">
         <v>24</v>
       </c>
@@ -2048,8 +2181,8 @@
       <c r="C15" s="37">
         <v>43338</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
       <c r="F15" s="38" t="s">
         <v>12</v>
       </c>
@@ -2098,10 +2231,10 @@
       <c r="C17" s="17">
         <v>43343</v>
       </c>
-      <c r="D17" s="70">
+      <c r="D17" s="68">
         <v>28</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F17" s="34" t="s">
@@ -2128,8 +2261,8 @@
       <c r="C18" s="51">
         <v>43343</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="38" t="s">
         <v>24</v>
       </c>
@@ -2150,8 +2283,8 @@
       <c r="C19" s="4">
         <v>43343</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="38" t="s">
         <v>12</v>
       </c>
@@ -2199,10 +2332,10 @@
       <c r="C21" s="18">
         <v>43334</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="68">
         <v>21</v>
       </c>
-      <c r="E21" s="70" t="s">
+      <c r="E21" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="34" t="s">
@@ -2229,8 +2362,8 @@
       <c r="C22" s="51">
         <v>43334</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="38" t="s">
         <v>24</v>
       </c>
@@ -2251,8 +2384,8 @@
       <c r="C23" s="51">
         <v>43334</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="38" t="s">
         <v>12</v>
       </c>
@@ -2300,10 +2433,10 @@
       <c r="C25" s="18">
         <v>43340</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="68">
         <v>24</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F25" s="34" t="s">
@@ -2315,7 +2448,7 @@
       <c r="H25" s="50">
         <v>45</v>
       </c>
-      <c r="I25" s="74" t="s">
+      <c r="I25" s="70" t="s">
         <v>21</v>
       </c>
       <c r="J25" s="50" t="s">
@@ -2330,8 +2463,8 @@
       <c r="C26" s="51">
         <v>43340</v>
       </c>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="38" t="s">
         <v>24</v>
       </c>
@@ -2341,7 +2474,7 @@
       <c r="H26" s="39">
         <v>2</v>
       </c>
-      <c r="I26" s="75"/>
+      <c r="I26" s="71"/>
       <c r="J26" s="24"/>
     </row>
     <row r="27" spans="1:10">
@@ -2352,7 +2485,7 @@
       <c r="C27" s="51">
         <v>43340</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="69"/>
       <c r="E27" s="26"/>
       <c r="F27" s="38" t="s">
         <v>12</v>
@@ -2401,10 +2534,10 @@
       <c r="C29" s="18">
         <v>43325</v>
       </c>
-      <c r="D29" s="70">
+      <c r="D29" s="68">
         <v>18</v>
       </c>
-      <c r="E29" s="70" t="s">
+      <c r="E29" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F29" s="34" t="s">
@@ -2431,8 +2564,8 @@
       <c r="C30" s="51">
         <v>43325</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
       <c r="F30" s="38" t="s">
         <v>24</v>
       </c>
@@ -2453,8 +2586,8 @@
       <c r="C31" s="51">
         <v>43325</v>
       </c>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="38" t="s">
         <v>12</v>
       </c>
@@ -2502,10 +2635,10 @@
       <c r="C33" s="18">
         <v>43302</v>
       </c>
-      <c r="D33" s="70">
+      <c r="D33" s="68">
         <v>6</v>
       </c>
-      <c r="E33" s="70" t="s">
+      <c r="E33" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F33" s="34" t="s">
@@ -2517,7 +2650,7 @@
       <c r="H33" s="50">
         <v>13</v>
       </c>
-      <c r="I33" s="68" t="s">
+      <c r="I33" s="74" t="s">
         <v>114</v>
       </c>
       <c r="J33" s="20" t="s">
@@ -2532,8 +2665,8 @@
       <c r="C34" s="51">
         <v>43302</v>
       </c>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="38" t="s">
         <v>12</v>
       </c>
@@ -2543,7 +2676,7 @@
       <c r="H34" s="39">
         <v>184</v>
       </c>
-      <c r="I34" s="69"/>
+      <c r="I34" s="75"/>
       <c r="J34" s="25"/>
     </row>
     <row r="35" spans="1:10">
@@ -2569,7 +2702,7 @@
       <c r="H35" s="39">
         <v>197</v>
       </c>
-      <c r="I35" s="69"/>
+      <c r="I35" s="75"/>
       <c r="J35" s="24"/>
     </row>
     <row r="36" spans="1:10">
@@ -2582,10 +2715,10 @@
       <c r="C36" s="18">
         <v>43316</v>
       </c>
-      <c r="D36" s="70">
+      <c r="D36" s="68">
         <v>12</v>
       </c>
-      <c r="E36" s="70" t="s">
+      <c r="E36" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F36" s="34" t="s">
@@ -2610,8 +2743,8 @@
       <c r="C37" s="51">
         <v>43320</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
       <c r="F37" s="38" t="s">
         <v>24</v>
       </c>
@@ -2632,8 +2765,8 @@
       <c r="C38" s="51">
         <v>43316</v>
       </c>
-      <c r="D38" s="71"/>
-      <c r="E38" s="71"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="38" t="s">
         <v>12</v>
       </c>
@@ -2681,10 +2814,10 @@
       <c r="C40" s="18">
         <v>43307</v>
       </c>
-      <c r="D40" s="70">
+      <c r="D40" s="68">
         <v>6</v>
       </c>
-      <c r="E40" s="70" t="s">
+      <c r="E40" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F40" s="34" t="s">
@@ -2696,7 +2829,7 @@
       <c r="H40" s="50">
         <v>32</v>
       </c>
-      <c r="I40" s="72" t="s">
+      <c r="I40" s="76" t="s">
         <v>26</v>
       </c>
       <c r="J40" s="58" t="s">
@@ -2711,8 +2844,8 @@
       <c r="C41" s="51">
         <v>43307</v>
       </c>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="38" t="s">
         <v>12</v>
       </c>
@@ -2722,7 +2855,7 @@
       <c r="H41" s="39">
         <v>268</v>
       </c>
-      <c r="I41" s="73"/>
+      <c r="I41" s="77"/>
       <c r="J41" s="59"/>
     </row>
     <row r="42" spans="1:10">
@@ -2746,7 +2879,7 @@
         <v>16</v>
       </c>
       <c r="H42" s="24"/>
-      <c r="I42" s="73"/>
+      <c r="I42" s="77"/>
       <c r="J42" s="59"/>
     </row>
     <row r="43" spans="1:10" ht="31.5">
@@ -2759,10 +2892,10 @@
       <c r="C43" s="18">
         <v>43344</v>
       </c>
-      <c r="D43" s="70">
+      <c r="D43" s="68">
         <v>14</v>
       </c>
-      <c r="E43" s="70" t="s">
+      <c r="E43" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F43" s="34" t="s">
@@ -2789,8 +2922,8 @@
       <c r="C44" s="51">
         <v>43335</v>
       </c>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
       <c r="F44" s="38" t="s">
         <v>24</v>
       </c>
@@ -2811,8 +2944,8 @@
       <c r="C45" s="51">
         <v>43344</v>
       </c>
-      <c r="D45" s="71"/>
-      <c r="E45" s="71"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
       <c r="F45" s="38" t="s">
         <v>12</v>
       </c>
@@ -2863,10 +2996,10 @@
       <c r="C47" s="18">
         <v>43325</v>
       </c>
-      <c r="D47" s="70">
+      <c r="D47" s="68">
         <v>16</v>
       </c>
-      <c r="E47" s="70" t="s">
+      <c r="E47" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F47" s="34" t="s">
@@ -2893,8 +3026,8 @@
       <c r="C48" s="51">
         <v>43325</v>
       </c>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
       <c r="F48" s="38" t="s">
         <v>24</v>
       </c>
@@ -2915,8 +3048,8 @@
       <c r="C49" s="51">
         <v>43325</v>
       </c>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
       <c r="F49" s="38" t="s">
         <v>12</v>
       </c>
@@ -2967,10 +3100,10 @@
       <c r="C51" s="18">
         <v>43338</v>
       </c>
-      <c r="D51" s="70">
+      <c r="D51" s="68">
         <v>17</v>
       </c>
-      <c r="E51" s="70" t="s">
+      <c r="E51" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F51" s="34" t="s">
@@ -2997,8 +3130,8 @@
       <c r="C52" s="51">
         <v>43331</v>
       </c>
-      <c r="D52" s="71"/>
-      <c r="E52" s="71"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
       <c r="F52" s="38" t="s">
         <v>24</v>
       </c>
@@ -3021,8 +3154,8 @@
       <c r="C53" s="51">
         <v>43338</v>
       </c>
-      <c r="D53" s="71"/>
-      <c r="E53" s="71"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
       <c r="F53" s="38" t="s">
         <v>12</v>
       </c>
@@ -3074,10 +3207,10 @@
       <c r="C55" s="18">
         <v>43316</v>
       </c>
-      <c r="D55" s="70">
+      <c r="D55" s="68">
         <v>11</v>
       </c>
-      <c r="E55" s="70" t="s">
+      <c r="E55" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F55" s="34" t="s">
@@ -3104,8 +3237,8 @@
       <c r="C56" s="51">
         <v>43316</v>
       </c>
-      <c r="D56" s="71"/>
-      <c r="E56" s="71"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
       <c r="F56" s="38" t="s">
         <v>12</v>
       </c>
@@ -3158,10 +3291,10 @@
       <c r="C58" s="18">
         <v>43330</v>
       </c>
-      <c r="D58" s="70">
+      <c r="D58" s="68">
         <v>19</v>
       </c>
-      <c r="E58" s="70" t="s">
+      <c r="E58" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F58" s="34" t="s">
@@ -3188,8 +3321,8 @@
       <c r="C59" s="51">
         <v>43322</v>
       </c>
-      <c r="D59" s="71"/>
-      <c r="E59" s="71"/>
+      <c r="D59" s="69"/>
+      <c r="E59" s="69"/>
       <c r="F59" s="38" t="s">
         <v>24</v>
       </c>
@@ -3212,8 +3345,8 @@
       <c r="C60" s="51">
         <v>43330</v>
       </c>
-      <c r="D60" s="71"/>
-      <c r="E60" s="71"/>
+      <c r="D60" s="69"/>
+      <c r="E60" s="69"/>
       <c r="F60" s="38" t="s">
         <v>12</v>
       </c>
@@ -3266,10 +3399,10 @@
       <c r="C62" s="18">
         <v>43334</v>
       </c>
-      <c r="D62" s="70">
+      <c r="D62" s="68">
         <v>16</v>
       </c>
-      <c r="E62" s="70" t="s">
+      <c r="E62" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F62" s="34" t="s">
@@ -3296,8 +3429,8 @@
       <c r="C63" s="51">
         <v>43320</v>
       </c>
-      <c r="D63" s="71"/>
-      <c r="E63" s="71"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="69"/>
       <c r="F63" s="38" t="s">
         <v>24</v>
       </c>
@@ -3320,8 +3453,8 @@
       <c r="C64" s="51">
         <v>43320</v>
       </c>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
+      <c r="D64" s="69"/>
+      <c r="E64" s="69"/>
       <c r="F64" s="38" t="s">
         <v>12</v>
       </c>
@@ -3374,10 +3507,10 @@
       <c r="C66" s="18">
         <v>43327</v>
       </c>
-      <c r="D66" s="70">
+      <c r="D66" s="68">
         <v>16</v>
       </c>
-      <c r="E66" s="70" t="s">
+      <c r="E66" s="68" t="s">
         <v>2</v>
       </c>
       <c r="F66" s="34" t="s">
@@ -3404,8 +3537,8 @@
       <c r="C67" s="51">
         <v>43319</v>
       </c>
-      <c r="D67" s="71"/>
-      <c r="E67" s="71"/>
+      <c r="D67" s="69"/>
+      <c r="E67" s="69"/>
       <c r="F67" s="38" t="s">
         <v>24</v>
       </c>
@@ -3428,8 +3561,8 @@
       <c r="C68" s="51">
         <v>43327</v>
       </c>
-      <c r="D68" s="71"/>
-      <c r="E68" s="71"/>
+      <c r="D68" s="69"/>
+      <c r="E68" s="69"/>
       <c r="F68" s="23" t="s">
         <v>12</v>
       </c>
@@ -3473,45 +3606,386 @@
       <c r="J69" s="67"/>
     </row>
     <row r="70" spans="1:10">
-      <c r="E70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="I70" s="9"/>
+      <c r="A70">
+        <v>2018</v>
+      </c>
+      <c r="B70" s="79">
+        <v>43255</v>
+      </c>
+      <c r="C70" s="79">
+        <v>43326</v>
+      </c>
+      <c r="D70" s="39">
+        <v>14</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70">
+        <f>547+37</f>
+        <v>584</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J70" s="38" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="71" spans="1:10">
-      <c r="E71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="I71" s="9"/>
+      <c r="B71" s="79">
+        <v>43297</v>
+      </c>
+      <c r="C71" s="80">
+        <v>43326</v>
+      </c>
+      <c r="D71" s="39">
+        <v>7</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G71" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71">
+        <f>69+1</f>
+        <v>70</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="72" spans="1:10">
-      <c r="G72" s="1"/>
-      <c r="I72" s="9"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="81">
+        <v>43283</v>
+      </c>
+      <c r="C72" s="81">
+        <v>43326</v>
+      </c>
+      <c r="D72" s="39">
+        <v>10</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G72" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H72" s="24">
+        <f>2947+205</f>
+        <v>3152</v>
+      </c>
+      <c r="I72" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J72" s="24"/>
     </row>
     <row r="73" spans="1:10">
-      <c r="G73" s="1"/>
-      <c r="I73" s="9"/>
+      <c r="A73" s="29"/>
+      <c r="B73" s="82">
+        <v>43297</v>
+      </c>
+      <c r="C73" s="83">
+        <v>43326</v>
+      </c>
+      <c r="D73" s="42">
+        <v>7</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H73" s="29">
+        <f>0+4296</f>
+        <v>4296</v>
+      </c>
+      <c r="I73" s="67" t="s">
+        <v>176</v>
+      </c>
+      <c r="J73" s="29"/>
     </row>
     <row r="74" spans="1:10">
-      <c r="G74" s="1"/>
-      <c r="I74" s="9"/>
+      <c r="A74" s="50">
+        <v>2019</v>
+      </c>
+      <c r="B74" s="84">
+        <v>43619</v>
+      </c>
+      <c r="C74" s="84">
+        <v>43680</v>
+      </c>
+      <c r="D74" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G74" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H74" s="50">
+        <f>29+5</f>
+        <v>34</v>
+      </c>
+      <c r="I74" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="19" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="75" spans="1:10">
-      <c r="G75" s="1"/>
-      <c r="I75" s="9"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="81">
+        <v>43660</v>
+      </c>
+      <c r="C75" s="80">
+        <v>43680</v>
+      </c>
+      <c r="D75" s="86" t="s">
+        <v>181</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F75" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G75" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H75" s="24">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="I75" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="J75" s="24"/>
     </row>
     <row r="76" spans="1:10">
-      <c r="G76" s="1"/>
-      <c r="I76" s="9"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="80">
+        <v>43647</v>
+      </c>
+      <c r="C76" s="81">
+        <v>43680</v>
+      </c>
+      <c r="D76" s="87" t="s">
+        <v>181</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G76" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="24">
+        <f>247+26</f>
+        <v>273</v>
+      </c>
+      <c r="I76" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J76" s="24"/>
     </row>
     <row r="77" spans="1:10">
-      <c r="G77" s="1"/>
-      <c r="I77" s="9"/>
+      <c r="A77" s="29"/>
+      <c r="B77" s="82">
+        <v>43661</v>
+      </c>
+      <c r="C77" s="83">
+        <v>43680</v>
+      </c>
+      <c r="D77" s="29">
+        <v>2</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" s="29">
+        <v>459</v>
+      </c>
+      <c r="I77" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="J77" s="29"/>
     </row>
     <row r="78" spans="1:10">
-      <c r="G78" s="1"/>
-      <c r="I78" s="9"/>
+      <c r="A78">
+        <v>2020</v>
+      </c>
+      <c r="B78" s="79">
+        <v>43997</v>
+      </c>
+      <c r="C78" s="79">
+        <v>44032</v>
+      </c>
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78">
+        <f>11 + 4</f>
+        <v>15</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="J78" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="B79" s="79">
+        <v>44032</v>
+      </c>
+      <c r="C79" s="79">
+        <v>44032</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="24"/>
+      <c r="B80" s="81">
+        <v>44015</v>
+      </c>
+      <c r="C80" s="81">
+        <v>44032</v>
+      </c>
+      <c r="D80" s="24">
+        <v>3</v>
+      </c>
+      <c r="E80" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F80" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="24">
+        <f>199+23</f>
+        <v>222</v>
+      </c>
+      <c r="I80" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="J80" s="24"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="29"/>
+      <c r="B81" s="82">
+        <v>44032</v>
+      </c>
+      <c r="C81" s="82">
+        <v>44032</v>
+      </c>
+      <c r="D81" s="29">
+        <v>1</v>
+      </c>
+      <c r="E81" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" s="29">
+        <v>72</v>
+      </c>
+      <c r="I81" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="J81" s="29"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="E82" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E13:E15"/>
     <mergeCell ref="E66:E68"/>
     <mergeCell ref="D66:D68"/>
     <mergeCell ref="D25:D27"/>
@@ -3526,29 +4000,6 @@
     <mergeCell ref="E58:E60"/>
     <mergeCell ref="E62:E64"/>
     <mergeCell ref="D62:D64"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3564,10 +4015,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <pane ySplit="4" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3580,7 +4032,7 @@
     <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>52</v>
       </c>
@@ -3588,7 +4040,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="48" thickBot="1">
+    <row r="4" spans="1:11" ht="48" thickBot="1">
       <c r="A4" s="56" t="s">
         <v>1</v>
       </c>
@@ -3619,8 +4071,11 @@
       <c r="J4" s="57" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="6" customFormat="1">
+      <c r="K4" s="88" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1">
       <c r="A5" s="15">
         <v>2001</v>
       </c>
@@ -3652,7 +4107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="B6" s="4">
         <v>43208</v>
@@ -3682,7 +4137,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="4">
         <v>43258</v>
@@ -3712,7 +4167,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="B8" s="4">
         <v>43258</v>
@@ -3742,7 +4197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" s="16">
         <v>2002</v>
       </c>
@@ -3774,7 +4229,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="2"/>
       <c r="B10" s="4">
         <v>43210</v>
@@ -3804,7 +4259,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="2"/>
       <c r="B11" s="4">
         <v>43259</v>
@@ -3834,7 +4289,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="2"/>
       <c r="B12" s="4">
         <v>43259</v>
@@ -3864,7 +4319,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="16">
         <v>2003</v>
       </c>
@@ -3896,7 +4351,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="2"/>
       <c r="B14" s="4">
         <v>43209</v>
@@ -3926,7 +4381,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="2"/>
       <c r="B15" s="4">
         <v>43258</v>
@@ -3956,7 +4411,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="2"/>
       <c r="B16" s="4">
         <v>43259</v>
@@ -4457,7 +4912,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:11">
       <c r="A33" s="2"/>
       <c r="B33" s="4">
         <v>43211</v>
@@ -4486,8 +4941,11 @@
       <c r="J33" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="2"/>
       <c r="B34" s="4">
         <v>43211</v>
@@ -4517,7 +4975,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:11">
       <c r="A35" s="2"/>
       <c r="B35" s="4">
         <v>43253</v>
@@ -4547,7 +5005,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:11">
       <c r="A36" s="2"/>
       <c r="B36" s="4">
         <v>43253</v>
@@ -4577,7 +5035,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" s="16">
         <v>2008</v>
       </c>
@@ -4609,7 +5067,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="31.5">
+    <row r="38" spans="1:11" ht="31.5">
       <c r="A38" s="2"/>
       <c r="B38" s="4">
         <v>43209</v>
@@ -4639,7 +5097,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="A39" s="2"/>
       <c r="B39" s="4">
         <v>43209</v>
@@ -4669,7 +5127,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:11">
       <c r="A40" s="2"/>
       <c r="B40" s="4">
         <v>43286</v>
@@ -4699,7 +5157,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41" s="2"/>
       <c r="B41" s="4">
         <v>43272</v>
@@ -4729,7 +5187,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42" s="16">
         <v>2009</v>
       </c>
@@ -4761,7 +5219,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:11">
       <c r="A43" s="2"/>
       <c r="B43" s="4">
         <v>43208</v>
@@ -4791,7 +5249,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44" s="2"/>
       <c r="B44" s="4">
         <v>43208</v>
@@ -4821,7 +5279,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45" s="2"/>
       <c r="B45" s="4">
         <v>43278</v>
@@ -4851,7 +5309,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:11">
       <c r="A46" s="2"/>
       <c r="B46" s="4">
         <v>43278</v>
@@ -4881,7 +5339,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="31.5">
+    <row r="47" spans="1:11" ht="31.5">
       <c r="A47" s="16">
         <v>2010</v>
       </c>
@@ -4913,7 +5371,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48" s="2"/>
       <c r="B48" s="4">
         <v>43267</v>
@@ -5400,7 +5858,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:11">
       <c r="A65" s="2"/>
       <c r="B65" s="4">
         <v>43208</v>
@@ -5430,7 +5888,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:11">
       <c r="A66" s="50">
         <v>2016</v>
       </c>
@@ -5462,7 +5920,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:11">
       <c r="A67" s="2"/>
       <c r="B67" s="4">
         <v>43234</v>
@@ -5492,7 +5950,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:11">
       <c r="A68" s="2"/>
       <c r="B68" s="4">
         <v>43206</v>
@@ -5512,7 +5970,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:11">
       <c r="A69" s="50">
         <v>2017</v>
       </c>
@@ -5544,7 +6002,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:11">
       <c r="B70" s="4">
         <v>43247</v>
       </c>
@@ -5573,20 +6031,21 @@
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
-      <c r="B71" s="4">
+    <row r="71" spans="1:11">
+      <c r="A71" s="24"/>
+      <c r="B71" s="51">
         <v>43261</v>
       </c>
-      <c r="C71" s="4">
+      <c r="C71" s="51">
         <v>43345</v>
       </c>
       <c r="D71" s="39">
         <v>7</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" s="23" t="s">
         <v>145</v>
       </c>
       <c r="G71" s="39">
@@ -5598,68 +6057,349 @@
       <c r="I71" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="J71" s="21" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="50"/>
-      <c r="B72" s="18">
+    <row r="72" spans="1:11">
+      <c r="A72" s="29"/>
+      <c r="B72" s="66">
         <v>43212</v>
       </c>
-      <c r="C72" s="18">
+      <c r="C72" s="66">
         <v>43359</v>
       </c>
-      <c r="D72" s="35">
+      <c r="D72" s="42">
         <v>3</v>
       </c>
-      <c r="E72" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="F72" s="19" t="s">
+      <c r="E72" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="G72" s="35">
+      <c r="G72" s="42">
         <v>320</v>
       </c>
-      <c r="H72" s="32" t="s">
+      <c r="H72" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="I72" s="58"/>
-      <c r="J72" s="16" t="s">
+      <c r="I72" s="67"/>
+      <c r="J72" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
+    <row r="73" spans="1:11">
+      <c r="A73">
+        <v>2018</v>
+      </c>
+      <c r="B73" s="79">
+        <v>43288</v>
+      </c>
+      <c r="C73" s="79">
+        <v>43330</v>
+      </c>
+      <c r="D73" s="39">
+        <v>7</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" s="39">
+        <v>0</v>
+      </c>
+      <c r="H73" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I73" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="J73" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="B74" s="79">
+        <v>43282</v>
+      </c>
+      <c r="C74" s="79">
+        <v>43386</v>
+      </c>
+      <c r="D74" s="39">
+        <v>7</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G74" s="39">
+        <v>1521</v>
+      </c>
+      <c r="H74" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I74" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="J74" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="B75" s="79">
+        <v>43240</v>
+      </c>
+      <c r="C75" s="79">
+        <v>43379</v>
+      </c>
+      <c r="D75" s="39">
+        <v>20</v>
+      </c>
+      <c r="E75" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F75" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G75" s="39">
+        <v>111</v>
+      </c>
+      <c r="H75" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I75" s="65" t="s">
+        <v>200</v>
+      </c>
+      <c r="J75" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="29"/>
+      <c r="B76" s="82">
+        <v>43261</v>
+      </c>
+      <c r="C76" s="82">
+        <v>43316</v>
+      </c>
+      <c r="D76" s="42">
+        <v>5</v>
+      </c>
+      <c r="E76" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F76" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G76" s="42">
+        <v>8</v>
+      </c>
+      <c r="H76" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I76" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="J76" s="40" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77">
+        <v>2019</v>
+      </c>
+      <c r="B77" s="79">
+        <v>43641</v>
+      </c>
+      <c r="C77" s="79">
+        <v>43678</v>
+      </c>
+      <c r="D77" s="39">
+        <v>3</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" s="39">
+        <v>0</v>
+      </c>
+      <c r="H77" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I77" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="J77" s="36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="B78" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="C78" s="79" t="s">
+        <v>184</v>
+      </c>
+      <c r="D78" t="s">
+        <v>181</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G78" s="39">
+        <v>71</v>
+      </c>
+      <c r="H78" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I78" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="J78" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="K78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="B79" s="80">
+        <v>43603</v>
+      </c>
+      <c r="C79" s="79">
+        <v>43680</v>
+      </c>
+      <c r="D79">
+        <v>10</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G79" s="39">
+        <v>57</v>
+      </c>
+      <c r="H79" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I79" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="J79" s="36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="29"/>
+      <c r="B80" s="82">
+        <v>43625</v>
+      </c>
+      <c r="C80" s="82">
+        <v>43673</v>
+      </c>
+      <c r="D80" s="29">
+        <v>6</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F80" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G80" s="42">
+        <v>34</v>
+      </c>
+      <c r="H80" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I80" s="78" t="s">
+        <v>187</v>
+      </c>
+      <c r="J80" s="40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81">
+        <v>2020</v>
+      </c>
+      <c r="B81" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" t="s">
+        <v>181</v>
+      </c>
+      <c r="E81" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F81" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="G81" s="39">
+        <v>571</v>
+      </c>
+      <c r="H81" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="I81" s="65" t="s">
+        <v>197</v>
+      </c>
+      <c r="J81" s="36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="29"/>
+      <c r="B82" s="82">
+        <v>44005</v>
+      </c>
+      <c r="C82" s="82">
+        <v>44058</v>
+      </c>
+      <c r="D82" s="29">
+        <v>12</v>
+      </c>
+      <c r="E82" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="F82" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="G82" s="42">
+        <v>37</v>
+      </c>
+      <c r="H82" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I82" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="J82" s="40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" t="s">
         <v>168</v>
       </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>